<commit_message>
annotations write to db and are compared to input file
</commit_message>
<xml_diff>
--- a/app/userData/sampleData.xlsx
+++ b/app/userData/sampleData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cscaudill/Documents/DataAnalyses/NLP/ModelTrainingUI/sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cscaudill/Documents/DataAnalyses/NLP/ModelTrainingUI/app_NoUpload/userData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE574BC-FC10-B24E-A682-A78E35CD1D24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774D136-1019-E246-8575-20290AA0A698}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{929CDC9E-8B6A-9145-A611-E89459EFFD59}"/>
   </bookViews>
@@ -30,16 +30,16 @@
     <t>XOM Description</t>
   </si>
   <si>
-    <t>DMP 08/08/16 QSNL - wrong product on four invoices 31103787,31103793 31103799, 31103804</t>
+    <t>Service Request Number</t>
   </si>
   <si>
-    <t>Tax being charged to invoice 9034520671 on ship to 154628. BU 10/04/2017 ***DUPLICATE SR***</t>
+    <t>Tax being charged to invoice 123456789 on ship to 987654321. BU 10/04/2017 ***DUPLICATE SR***</t>
   </si>
   <si>
-    <t>At 3.30AM, driver, Anthony called, said that his VC number doesn't work. CS checked in SAP, everything seems to be normal  CS checked in Omega, it appears that the Volume contract number 99237 disappeared from Omega. Therefore, the error message in Journal was "Drawer Not Found". CS reposted the VC 99237 from SAP and waited for 15 Mins but itstill does not appear in Omega. Therefore, CS granted the manual load number, in order for the driver to be able to load the product as soon as possible. The driver required 36,000L of ADO and 3,000L of ULP. The NEW shipment number is 105915713</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum</t>
   </si>
   <si>
-    <t>Service Request Number</t>
+    <t>CSC 08/08/16 ABCD - wrong product on four invoices 12345, 67890, 09876, 54321</t>
   </si>
 </sst>
 </file>
@@ -394,14 +394,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -409,15 +409,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>27005</v>
+        <v>12345</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20166</v>
+        <v>67890</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>79553</v>
+        <v>54321</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>

</xml_diff>